<commit_message>
sao cứ để 1899 hoài vậy
</commit_message>
<xml_diff>
--- a/src/public/exports/hopdonggvmList.xlsx
+++ b/src/public/exports/hopdonggvmList.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Ngày Bắt Đầu</t>
   </si>
@@ -88,10 +88,43 @@
     <t>Ông</t>
   </si>
   <si>
-    <t>Dương Văn Mạnh</t>
-  </si>
-  <si>
-    <t>035078000000</t>
+    <t>Lê Văn Mạnh</t>
+  </si>
+  <si>
+    <t>00120300214</t>
+  </si>
+  <si>
+    <t>Hà Nội</t>
+  </si>
+  <si>
+    <t>Taidz05@gmail.com</t>
+  </si>
+  <si>
+    <t>Thạc sĩ</t>
+  </si>
+  <si>
+    <t>giảng viên</t>
+  </si>
+  <si>
+    <t>01244211003</t>
+  </si>
+  <si>
+    <t>mb bank</t>
+  </si>
+  <si>
+    <t>Bốn  Triệu Bảy Trăm Không Mươi Nghìn Không Trăm Đồng</t>
+  </si>
+  <si>
+    <t>Bốn Trăm Bảy Mươi Nghìn Không Trăm Đồng</t>
+  </si>
+  <si>
+    <t>Bốn  Triệu Hai Trăm Ba Mươi Nghìn Không Trăm Đồng</t>
+  </si>
+  <si>
+    <t>Nguyễn Hoàng Minh An</t>
+  </si>
+  <si>
+    <t>035078000253</t>
   </si>
   <si>
     <t>CCSĐKQLCTVDLQGVDC</t>
@@ -100,7 +133,10 @@
     <t>huudq@tmu.edu.vn</t>
   </si>
   <si>
-    <t/>
+    <t>Tiến sĩ</t>
+  </si>
+  <si>
+    <t>Giảng viên</t>
   </si>
   <si>
     <t>22010000163 915</t>
@@ -109,43 +145,13 @@
     <t>BIDV, chi nhánh Thăng Long</t>
   </si>
   <si>
-    <t>Sáu  Triệu Năm Trăm Không Mươi Nghìn Không Trăm Đồng</t>
-  </si>
-  <si>
-    <t>Sáu Trăm Lăm Nghìn Không Trăm Đồng</t>
-  </si>
-  <si>
-    <t>Năm  Triệu Tám Trăm Lăm Nghìn Không Trăm Đồng</t>
-  </si>
-  <si>
-    <t>Đặng Thị Kim Anh</t>
-  </si>
-  <si>
-    <t>00207800098003</t>
-  </si>
-  <si>
-    <t>Mười Triệu Không Trăm Nghìn Không Trăm Đồng</t>
-  </si>
-  <si>
-    <t>Một  Triệu Không Trăm Nghìn Không Trăm Đồng</t>
-  </si>
-  <si>
-    <t>Chín  Triệu Không Trăm Nghìn Không Trăm Đồng</t>
-  </si>
-  <si>
-    <t>Đoàn Minh Phương</t>
-  </si>
-  <si>
-    <t>035078000508</t>
-  </si>
-  <si>
-    <t>Mười Triệu Tám Trăm Không Mươi Nghìn Không Trăm Đồng</t>
-  </si>
-  <si>
-    <t>Một  Triệu Không Trăm Tám Mươi Nghìn Không Trăm Đồng</t>
-  </si>
-  <si>
-    <t>Chín  Triệu Bảy Trăm Hai Mươi Nghìn Không Trăm Đồng</t>
+    <t>Chín  Triệu Bốn Trăm Không Mươi Nghìn Không Trăm Đồng</t>
+  </si>
+  <si>
+    <t>Chín Trăm Bốn Mươi Nghìn Không Trăm Đồng</t>
+  </si>
+  <si>
+    <t>Tám  Triệu Bốn Trăm Sáu Mươi Nghìn Không Trăm Đồng</t>
   </si>
 </sst>
 </file>
@@ -537,7 +543,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X4"/>
+  <dimension ref="A1:X3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="15" customWidth="1"/>
@@ -636,12 +642,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>45563.70833333333</v>
-      </c>
+    <row r="2" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B2" s="2">
-        <v>45594.70833333333</v>
+        <v>-30.279212962963356</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
@@ -653,7 +656,7 @@
         <v>25</v>
       </c>
       <c r="F2" s="2">
-        <v>28531.708333333332</v>
+        <v>45573.70833333333</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>26</v>
@@ -665,57 +668,54 @@
         <v>28</v>
       </c>
       <c r="J2" s="3">
-        <v>2147483647</v>
+        <v>44444</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>29</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M2" s="3">
-        <v>4</v>
+        <v>4.400000095367432</v>
       </c>
       <c r="N2" s="3">
-        <v>988710727</v>
+        <v>33195343</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q2" s="3">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="R2" s="3">
-        <v>6500000</v>
+        <v>4700000</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T2" s="3">
-        <v>650000</v>
+        <v>470000</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="V2" s="3">
-        <v>5850000</v>
+        <v>4230000</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="X2" s="2">
-        <v>NaN</v>
+        <v>-30.279212962963356</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>45563.70833333333</v>
-      </c>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
-        <v>45594.70833333333</v>
+        <v>-30.279212962963356</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -724,28 +724,28 @@
         <v>24</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F3" s="2">
-        <v>28532.708333333332</v>
+        <v>28528.708333333332</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="J3" s="3">
         <v>2147483647</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="M3" s="3">
         <v>4</v>
@@ -754,108 +754,34 @@
         <v>988710727</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="Q3" s="3">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="R3" s="3">
-        <v>10000000</v>
+        <v>9400000</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="T3" s="3">
-        <v>1000000</v>
+        <v>940000</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="V3" s="3">
-        <v>9000000</v>
+        <v>8460000</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="X3" s="2">
-        <v>NaN</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>45563.70833333333</v>
-      </c>
-      <c r="B4" s="2">
-        <v>45594.70833333333</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="2">
-        <v>28528.708333333332</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="3">
-        <v>2147483647</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="3">
-        <v>4</v>
-      </c>
-      <c r="N4" s="3">
-        <v>988710727</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q4" s="3">
-        <v>108</v>
-      </c>
-      <c r="R4" s="3">
-        <v>10800000</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="T4" s="3">
-        <v>1080000</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="V4" s="3">
-        <v>9720000</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="X4" s="2">
-        <v>NaN</v>
+        <v>-30.279212962963356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
đổi lại sql xuất hợp đồng tất cả trừ xuất docx theo tên
</commit_message>
<xml_diff>
--- a/src/public/exports/hopdonggvmList.xlsx
+++ b/src/public/exports/hopdonggvmList.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
   <si>
     <t>Ngày Bắt Đầu</t>
   </si>
@@ -37,6 +37,9 @@
     <t>Nơi Cấp CCCD</t>
   </si>
   <si>
+    <t>Địa Chỉ Theo CCCD</t>
+  </si>
+  <si>
     <t>Email</t>
   </si>
   <si>
@@ -95,6 +98,9 @@
   </si>
   <si>
     <t>CCSĐKQLCTVDLQGVDC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mai Dịch, Cầu Giấy, </t>
   </si>
   <si>
     <t>huudq@tmu.edu.vn</t>
@@ -548,21 +554,22 @@
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="25" customWidth="1"/>
-    <col min="10" max="10" width="15" customWidth="1"/>
-    <col min="11" max="11" width="10" customWidth="1"/>
-    <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="15" width="15" customWidth="1"/>
-    <col min="16" max="16" width="20" customWidth="1"/>
-    <col min="17" max="17" width="10" customWidth="1"/>
-    <col min="18" max="18" width="15" customWidth="1"/>
-    <col min="19" max="19" width="30" customWidth="1"/>
-    <col min="20" max="20" width="15" customWidth="1"/>
-    <col min="21" max="21" width="30" customWidth="1"/>
-    <col min="22" max="22" width="15" customWidth="1"/>
-    <col min="23" max="23" width="30" customWidth="1"/>
-    <col min="24" max="25" width="15" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="10" max="10" width="25" customWidth="1"/>
+    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="10" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
+    <col min="14" max="14" width="10" customWidth="1"/>
+    <col min="15" max="16" width="15" customWidth="1"/>
+    <col min="17" max="17" width="20" customWidth="1"/>
+    <col min="18" max="18" width="10" customWidth="1"/>
+    <col min="19" max="19" width="15" customWidth="1"/>
+    <col min="20" max="20" width="30" customWidth="1"/>
+    <col min="21" max="21" width="15" customWidth="1"/>
+    <col min="22" max="22" width="30" customWidth="1"/>
+    <col min="23" max="23" width="15" customWidth="1"/>
+    <col min="24" max="24" width="30" customWidth="1"/>
+    <col min="25" max="25" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -639,7 +646,7 @@
         <v>23</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -653,64 +660,67 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F2" s="2">
         <v>28530.708333333332</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="3">
+        <v>29</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="3">
         <v>2147483647</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="L2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" s="3">
+        <v>31</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="3">
         <v>4</v>
       </c>
-      <c r="N2" s="3">
+      <c r="O2" s="3">
         <v>988710727</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="P2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q2" s="3">
+        <v>33</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" s="3">
         <v>110</v>
       </c>
-      <c r="R2" s="3">
+      <c r="S2" s="3">
         <v>11000000</v>
       </c>
-      <c r="S2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="T2" s="3">
+      <c r="T2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="U2" s="3">
         <v>1100000</v>
       </c>
-      <c r="U2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="V2" s="3">
+      <c r="V2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="3">
         <v>9900000</v>
       </c>
-      <c r="W2" s="3" t="s">
-        <v>35</v>
+      <c r="X2" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="Y2" s="2">
         <v>45597.70833333333</v>
@@ -727,64 +737,67 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F3" s="2">
         <v>28532.708333333332</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="3">
+        <v>29</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="3">
         <v>2147483647</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="L3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3" s="3">
+        <v>31</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="3">
         <v>4</v>
       </c>
-      <c r="N3" s="3">
+      <c r="O3" s="3">
         <v>988710727</v>
       </c>
-      <c r="O3" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="P3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q3" s="3">
+        <v>33</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" s="3">
         <v>100</v>
       </c>
-      <c r="R3" s="3">
+      <c r="S3" s="3">
         <v>10000000</v>
       </c>
-      <c r="S3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="T3" s="3">
+      <c r="T3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="U3" s="3">
         <v>1000000</v>
       </c>
-      <c r="U3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="V3" s="3">
+      <c r="V3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="W3" s="3">
         <v>9000000</v>
       </c>
-      <c r="W3" s="3" t="s">
-        <v>40</v>
+      <c r="X3" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="Y3" s="2">
         <v>45597.70833333333</v>
@@ -801,64 +814,67 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F4" s="2">
         <v>28528.708333333332</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="3">
+        <v>29</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="3">
         <v>2147483647</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="L4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" s="3">
+        <v>31</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" s="3">
         <v>4</v>
       </c>
-      <c r="N4" s="3">
+      <c r="O4" s="3">
         <v>988710727</v>
       </c>
-      <c r="O4" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="P4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q4" s="3">
+        <v>33</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="R4" s="3">
         <v>314</v>
       </c>
-      <c r="R4" s="3">
+      <c r="S4" s="3">
         <v>31400000</v>
       </c>
-      <c r="S4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="T4" s="3">
+      <c r="T4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="U4" s="3">
         <v>3140000</v>
       </c>
-      <c r="U4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="V4" s="3">
+      <c r="V4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="W4" s="3">
         <v>28260000</v>
       </c>
-      <c r="W4" s="3" t="s">
-        <v>45</v>
+      <c r="X4" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="Y4" s="2">
         <v>45598.70833333333</v>

</xml_diff>

<commit_message>
chỉnh lại duyệt bên đào tạo
</commit_message>
<xml_diff>
--- a/src/public/exports/hopdonggvmList.xlsx
+++ b/src/public/exports/hopdonggvmList.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t>Ngày Bắt Đầu</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>CCSĐKQLCTVDLQGVDC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mai Dịch, Cầu Giấy, </t>
   </si>
   <si>
     <t>huudq@tmu.edu.vn</t>
@@ -674,20 +671,17 @@
       <c r="H2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="K2" s="3">
         <v>2147483647</v>
       </c>
       <c r="L2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="N2" s="3">
         <v>4</v>
@@ -696,10 +690,10 @@
         <v>988710727</v>
       </c>
       <c r="P2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="R2" s="3">
         <v>110</v>
@@ -708,19 +702,19 @@
         <v>11000000</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U2" s="3">
         <v>1100000</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="W2" s="3">
         <v>9900000</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Y2" s="2">
         <v>45597.70833333333</v>
@@ -740,31 +734,28 @@
         <v>25</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F3" s="2">
         <v>28532.708333333332</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="K3" s="3">
         <v>2147483647</v>
       </c>
       <c r="L3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="N3" s="3">
         <v>4</v>
@@ -773,10 +764,10 @@
         <v>988710727</v>
       </c>
       <c r="P3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="R3" s="3">
         <v>100</v>
@@ -785,19 +776,19 @@
         <v>10000000</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U3" s="3">
         <v>1000000</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W3" s="3">
         <v>9000000</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Y3" s="2">
         <v>45597.70833333333</v>
@@ -817,31 +808,28 @@
         <v>25</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" s="2">
         <v>28528.708333333332</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="K4" s="3">
         <v>2147483647</v>
       </c>
       <c r="L4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="N4" s="3">
         <v>4</v>
@@ -850,10 +838,10 @@
         <v>988710727</v>
       </c>
       <c r="P4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="R4" s="3">
         <v>314</v>
@@ -862,19 +850,19 @@
         <v>31400000</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="U4" s="3">
         <v>3140000</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="W4" s="3">
         <v>28260000</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Y4" s="2">
         <v>45598.70833333333</v>

</xml_diff>

<commit_message>
chỉnh sửa lỗi do lệch múi giờ bên thông tin hợp đồng (infoHDGvm)
</commit_message>
<xml_diff>
--- a/src/public/exports/hopdonggvmList.xlsx
+++ b/src/public/exports/hopdonggvmList.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="68">
   <si>
     <t>Ngày Bắt Đầu</t>
   </si>
@@ -88,18 +88,30 @@
     <t>Ngày Nghiệm Thu</t>
   </si>
   <si>
+    <t>3/12/2024</t>
+  </si>
+  <si>
+    <t>6/12/2024</t>
+  </si>
+  <si>
     <t>Ông</t>
   </si>
   <si>
     <t>Bùi Thị Như</t>
   </si>
   <si>
+    <t>10/2/1978</t>
+  </si>
+  <si>
     <t>03507800058002</t>
   </si>
   <si>
     <t>CCSĐKQLCTVDLQGVDC</t>
   </si>
   <si>
+    <t xml:space="preserve">Mai Dịch, Cầu Giấy, </t>
+  </si>
+  <si>
     <t>huudq@tmu.edu.vn</t>
   </si>
   <si>
@@ -124,9 +136,30 @@
     <t>Chín  Triệu Chín Trăm Không Mươi Nghìn Không Trăm Đồng</t>
   </si>
   <si>
+    <t>Dương Văn Mạnh</t>
+  </si>
+  <si>
+    <t>11/2/1978</t>
+  </si>
+  <si>
+    <t>035078000000</t>
+  </si>
+  <si>
+    <t>Sáu  Triệu Năm Trăm Không Mươi Nghìn Không Trăm Đồng</t>
+  </si>
+  <si>
+    <t>Sáu Trăm Lăm Nghìn Không Trăm Đồng</t>
+  </si>
+  <si>
+    <t>Năm  Triệu Tám Trăm Lăm Nghìn Không Trăm Đồng</t>
+  </si>
+  <si>
     <t>Đặng Thị Kim Anh</t>
   </si>
   <si>
+    <t>12/2/1978</t>
+  </si>
+  <si>
     <t>00207800098003</t>
   </si>
   <si>
@@ -139,19 +172,49 @@
     <t>Chín  Triệu Không Trăm Nghìn Không Trăm Đồng</t>
   </si>
   <si>
+    <t>Đỗ Thái Dương</t>
+  </si>
+  <si>
+    <t>31/10/2024</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Hà Nội</t>
+  </si>
+  <si>
+    <t>huedm.c3chuyen@thainguyen.edu.vn</t>
+  </si>
+  <si>
+    <t>Thạc sĩ</t>
+  </si>
+  <si>
+    <t>giảng viên</t>
+  </si>
+  <si>
+    <t>0325266412</t>
+  </si>
+  <si>
+    <t>mb bank</t>
+  </si>
+  <si>
+    <t>Bốn  Triệu Ba Trăm Không Mươi Nghìn Không Trăm Đồng</t>
+  </si>
+  <si>
+    <t>Bốn Trăm Ba Mươi Nghìn Không Trăm Đồng</t>
+  </si>
+  <si>
+    <t>Ba  Triệu Tám Trăm Bảy Mươi Nghìn Không Trăm Đồng</t>
+  </si>
+  <si>
     <t>Đoàn Minh Phương</t>
   </si>
   <si>
+    <t>8/2/1978</t>
+  </si>
+  <si>
     <t>035078000508</t>
-  </si>
-  <si>
-    <t>Ba Mươi Một  Triệu Bốn Trăm Không Mươi Nghìn Không Trăm Đồng</t>
-  </si>
-  <si>
-    <t>Ba  Triệu Một Trăm Bốn Mươi Nghìn Không Trăm Đồng</t>
-  </si>
-  <si>
-    <t>Hai Mươi Tám  Triệu Hai Trăm Sáu Mươi Nghìn Không Trăm Đồng</t>
   </si>
 </sst>
 </file>
@@ -197,12 +260,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -543,7 +605,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:Y6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="15" customWidth="1"/>
@@ -647,225 +709,388 @@
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>45596.70833333333</v>
-      </c>
-      <c r="B2" s="2">
-        <v>45597.70833333333</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="2">
+        <v>2147483647</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="2">
+        <v>4</v>
+      </c>
+      <c r="O2" s="2">
+        <v>988710727</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R2" s="2">
+        <v>110</v>
+      </c>
+      <c r="S2" s="2">
+        <v>11000000</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" s="2">
+        <v>1100000</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="W2" s="2">
+        <v>9900000</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="F2" s="2">
-        <v>28530.708333333332</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="3">
-        <v>2147483647</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" s="3">
-        <v>4</v>
-      </c>
-      <c r="O2" s="3">
-        <v>988710727</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="R2" s="3">
-        <v>110</v>
-      </c>
-      <c r="S2" s="3">
-        <v>11000000</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="U2" s="3">
-        <v>1100000</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="W2" s="3">
-        <v>9900000</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y2" s="2">
-        <v>45597.70833333333</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>45596.70833333333</v>
-      </c>
-      <c r="B3" s="2">
-        <v>45597.70833333333</v>
-      </c>
-      <c r="C3" s="3">
+      <c r="A3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="2">
+        <v>2147483647</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="2">
+        <v>4</v>
+      </c>
+      <c r="O3" s="2">
+        <v>988710727</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="2">
-        <v>28532.708333333332</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" s="3">
-        <v>2147483647</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="N3" s="3">
-        <v>4</v>
-      </c>
-      <c r="O3" s="3">
-        <v>988710727</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="R3" s="3">
-        <v>100</v>
-      </c>
-      <c r="S3" s="3">
-        <v>10000000</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="U3" s="3">
-        <v>1000000</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="W3" s="3">
-        <v>9000000</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y3" s="2">
-        <v>45597.70833333333</v>
+      <c r="R3" s="2">
+        <v>65</v>
+      </c>
+      <c r="S3" s="2">
+        <v>6500000</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="U3" s="2">
+        <v>650000</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="W3" s="2">
+        <v>5850000</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>45596.70833333333</v>
-      </c>
-      <c r="B4" s="2">
-        <v>45598.70833333333</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="A4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="2">
+        <v>2147483647</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="2">
+        <v>4</v>
+      </c>
+      <c r="O4" s="2">
+        <v>988710727</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" s="2">
+        <v>100</v>
+      </c>
+      <c r="S4" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U4" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W4" s="2">
+        <v>9000000</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="2">
-        <v>28528.708333333332</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="B5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="N5" s="2">
+        <v>4</v>
+      </c>
+      <c r="O5" s="2">
+        <v>334553232</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="R5" s="2">
         <v>43</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" s="3">
+      <c r="S5" s="2">
+        <v>4300000</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="U5" s="2">
+        <v>430000</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="W5" s="2">
+        <v>3870000</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="2">
         <v>2147483647</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4" s="3">
+      <c r="L6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N6" s="2">
         <v>4</v>
       </c>
-      <c r="O4" s="3">
+      <c r="O6" s="2">
         <v>988710727</v>
       </c>
-      <c r="P4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="R4" s="3">
-        <v>314</v>
-      </c>
-      <c r="S4" s="3">
-        <v>31400000</v>
-      </c>
-      <c r="T4" s="3" t="s">
+      <c r="P6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R6" s="2">
+        <v>65</v>
+      </c>
+      <c r="S6" s="2">
+        <v>6500000</v>
+      </c>
+      <c r="T6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="U4" s="3">
-        <v>3140000</v>
-      </c>
-      <c r="V4" s="3" t="s">
+      <c r="U6" s="2">
+        <v>650000</v>
+      </c>
+      <c r="V6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="W4" s="3">
-        <v>28260000</v>
-      </c>
-      <c r="X4" s="3" t="s">
+      <c r="W6" s="2">
+        <v>5850000</v>
+      </c>
+      <c r="X6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="Y4" s="2">
-        <v>45598.70833333333</v>
+      <c r="Y6" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix copy ngày bên site info1
</commit_message>
<xml_diff>
--- a/src/public/exports/hopdonggvmList.xlsx
+++ b/src/public/exports/hopdonggvmList.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="68">
   <si>
     <t>Ngày Bắt Đầu</t>
   </si>
@@ -88,10 +88,10 @@
     <t>Ngày Nghiệm Thu</t>
   </si>
   <si>
-    <t>3/12/2024</t>
-  </si>
-  <si>
-    <t>6/12/2024</t>
+    <t>5/8/2024</t>
+  </si>
+  <si>
+    <t>8/12/2024</t>
   </si>
   <si>
     <t>Ông</t>
@@ -136,13 +136,67 @@
     <t>Chín  Triệu Chín Trăm Không Mươi Nghìn Không Trăm Đồng</t>
   </si>
   <si>
-    <t>Dương Văn Mạnh</t>
-  </si>
-  <si>
-    <t>11/2/1978</t>
-  </si>
-  <si>
-    <t>035078000000</t>
+    <t>Nguyễn Hoàng Minh An</t>
+  </si>
+  <si>
+    <t>7/2/1978</t>
+  </si>
+  <si>
+    <t>035078000253</t>
+  </si>
+  <si>
+    <t>Bốn  Triệu Ba Trăm Không Mươi Nghìn Không Trăm Đồng</t>
+  </si>
+  <si>
+    <t>Bốn Trăm Ba Mươi Nghìn Không Trăm Đồng</t>
+  </si>
+  <si>
+    <t>Ba  Triệu Tám Trăm Bảy Mươi Nghìn Không Trăm Đồng</t>
+  </si>
+  <si>
+    <t>Đặng Thị Kim Anh</t>
+  </si>
+  <si>
+    <t>12/2/1978</t>
+  </si>
+  <si>
+    <t>00207800098003</t>
+  </si>
+  <si>
+    <t>Mười Triệu Không Trăm Nghìn Không Trăm Đồng</t>
+  </si>
+  <si>
+    <t>Một  Triệu Không Trăm Nghìn Không Trăm Đồng</t>
+  </si>
+  <si>
+    <t>Chín  Triệu Không Trăm Nghìn Không Trăm Đồng</t>
+  </si>
+  <si>
+    <t>Đỗ Thái Dương</t>
+  </si>
+  <si>
+    <t>30/10/2024</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Hà Nội</t>
+  </si>
+  <si>
+    <t>huedm.c3chuyen@thainguyen.edu.vn</t>
+  </si>
+  <si>
+    <t>Thạc sĩ</t>
+  </si>
+  <si>
+    <t>giảng viên</t>
+  </si>
+  <si>
+    <t>0325266412</t>
+  </si>
+  <si>
+    <t>mb bank</t>
   </si>
   <si>
     <t>Sáu  Triệu Năm Trăm Không Mươi Nghìn Không Trăm Đồng</t>
@@ -154,106 +208,10 @@
     <t>Năm  Triệu Tám Trăm Lăm Nghìn Không Trăm Đồng</t>
   </si>
   <si>
-    <t>20/11/2024</t>
-  </si>
-  <si>
-    <t>Lê Văn Mạnh</t>
-  </si>
-  <si>
-    <t>9/10/2024</t>
-  </si>
-  <si>
-    <t>00120300214</t>
-  </si>
-  <si>
-    <t>Hà Nội</t>
-  </si>
-  <si>
-    <t>Taidz05@gmail.com</t>
-  </si>
-  <si>
-    <t>Thạc sĩ</t>
-  </si>
-  <si>
-    <t>giảng viên</t>
-  </si>
-  <si>
-    <t>01244211003</t>
-  </si>
-  <si>
-    <t>mb bank</t>
-  </si>
-  <si>
-    <t>Chín  Triệu Bốn Trăm Không Mươi Nghìn Không Trăm Đồng</t>
-  </si>
-  <si>
-    <t>Chín Trăm Bốn Mươi Nghìn Không Trăm Đồng</t>
-  </si>
-  <si>
-    <t>Tám  Triệu Bốn Trăm Sáu Mươi Nghìn Không Trăm Đồng</t>
-  </si>
-  <si>
-    <t>Nguyễn Hoàng Minh An</t>
+    <t>Đoàn Minh Phương</t>
   </si>
   <si>
     <t>8/2/1978</t>
-  </si>
-  <si>
-    <t>035078000253</t>
-  </si>
-  <si>
-    <t>Bốn  Triệu Bảy Trăm Không Mươi Nghìn Không Trăm Đồng</t>
-  </si>
-  <si>
-    <t>Bốn Trăm Bảy Mươi Nghìn Không Trăm Đồng</t>
-  </si>
-  <si>
-    <t>Bốn  Triệu Hai Trăm Ba Mươi Nghìn Không Trăm Đồng</t>
-  </si>
-  <si>
-    <t>Đặng Thị Kim Anh</t>
-  </si>
-  <si>
-    <t>12/2/1978</t>
-  </si>
-  <si>
-    <t>00207800098003</t>
-  </si>
-  <si>
-    <t>Mười Triệu Không Trăm Nghìn Không Trăm Đồng</t>
-  </si>
-  <si>
-    <t>Một  Triệu Không Trăm Nghìn Không Trăm Đồng</t>
-  </si>
-  <si>
-    <t>Chín  Triệu Không Trăm Nghìn Không Trăm Đồng</t>
-  </si>
-  <si>
-    <t>Đỗ Thái Dương</t>
-  </si>
-  <si>
-    <t>31/10/2024</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>huedm.c3chuyen@thainguyen.edu.vn</t>
-  </si>
-  <si>
-    <t>0325266412</t>
-  </si>
-  <si>
-    <t>Bốn  Triệu Ba Trăm Không Mươi Nghìn Không Trăm Đồng</t>
-  </si>
-  <si>
-    <t>Bốn Trăm Ba Mươi Nghìn Không Trăm Đồng</t>
-  </si>
-  <si>
-    <t>Ba  Triệu Tám Trăm Bảy Mươi Nghìn Không Trăm Đồng</t>
-  </si>
-  <si>
-    <t>Đoàn Minh Phương</t>
   </si>
   <si>
     <t>035078000508</t>
@@ -647,7 +605,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y8"/>
+  <dimension ref="A1:Y6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="15" customWidth="1"/>
@@ -880,22 +838,22 @@
         <v>37</v>
       </c>
       <c r="R3" s="2">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="S3" s="2">
-        <v>6500000</v>
+        <v>4300000</v>
       </c>
       <c r="T3" s="2" t="s">
         <v>44</v>
       </c>
       <c r="U3" s="2">
-        <v>650000</v>
+        <v>430000</v>
       </c>
       <c r="V3" s="2" t="s">
         <v>45</v>
       </c>
       <c r="W3" s="2">
-        <v>5850000</v>
+        <v>3870000</v>
       </c>
       <c r="X3" s="2" t="s">
         <v>46</v>
@@ -906,10 +864,10 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -918,75 +876,75 @@
         <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="2">
+        <v>2147483647</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="2">
+        <v>4</v>
+      </c>
+      <c r="O4" s="2">
+        <v>988710727</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" s="2">
+        <v>100</v>
+      </c>
+      <c r="S4" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="T4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="U4" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="V4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J4" s="2" t="s">
+      <c r="W4" s="2">
+        <v>9000000</v>
+      </c>
+      <c r="X4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="K4" s="2">
-        <v>44444</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="N4" s="2">
-        <v>4.400000095367432</v>
-      </c>
-      <c r="O4" s="2">
-        <v>33195343</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="R4" s="2">
-        <v>94</v>
-      </c>
-      <c r="S4" s="2">
-        <v>9400000</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="U4" s="2">
-        <v>940000</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="W4" s="2">
-        <v>8460000</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="Y4" s="2" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -995,67 +953,67 @@
         <v>27</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="K5" s="2">
-        <v>2147483647</v>
+        <v>0</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="N5" s="2">
         <v>4</v>
       </c>
       <c r="O5" s="2">
-        <v>988710727</v>
+        <v>334553232</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="R5" s="2">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="S5" s="2">
-        <v>4700000</v>
+        <v>6500000</v>
       </c>
       <c r="T5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="U5" s="2">
+        <v>650000</v>
+      </c>
+      <c r="V5" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="U5" s="2">
-        <v>470000</v>
-      </c>
-      <c r="V5" s="2" t="s">
+      <c r="W5" s="2">
+        <v>5850000</v>
+      </c>
+      <c r="X5" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="W5" s="2">
-        <v>4230000</v>
-      </c>
-      <c r="X5" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="Y5" s="2" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -1072,13 +1030,13 @@
         <v>27</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>31</v>
@@ -1111,181 +1069,27 @@
         <v>37</v>
       </c>
       <c r="R6" s="2">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="S6" s="2">
-        <v>10000000</v>
+        <v>6500000</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="U6" s="2">
-        <v>1000000</v>
+        <v>650000</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="W6" s="2">
-        <v>9000000</v>
+        <v>5850000</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K7" s="2">
-        <v>0</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="N7" s="2">
-        <v>4</v>
-      </c>
-      <c r="O7" s="2">
-        <v>334553232</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="R7" s="2">
-        <v>43</v>
-      </c>
-      <c r="S7" s="2">
-        <v>4300000</v>
-      </c>
-      <c r="T7" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="U7" s="2">
-        <v>430000</v>
-      </c>
-      <c r="V7" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="W7" s="2">
-        <v>3870000</v>
-      </c>
-      <c r="X7" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="Y7" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" s="2">
-        <v>2147483647</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N8" s="2">
-        <v>4</v>
-      </c>
-      <c r="O8" s="2">
-        <v>988710727</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="R8" s="2">
-        <v>65</v>
-      </c>
-      <c r="S8" s="2">
-        <v>6500000</v>
-      </c>
-      <c r="T8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="U8" s="2">
-        <v>650000</v>
-      </c>
-      <c r="V8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="W8" s="2">
-        <v>5850000</v>
-      </c>
-      <c r="X8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y8" s="2" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix chèn ngày bên mời giảng
</commit_message>
<xml_diff>
--- a/src/public/exports/hopdonggvmList.xlsx
+++ b/src/public/exports/hopdonggvmList.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="70">
   <si>
     <t>Ngày Bắt Đầu</t>
   </si>
@@ -88,10 +88,10 @@
     <t>Ngày Nghiệm Thu</t>
   </si>
   <si>
-    <t>3/12/2024</t>
-  </si>
-  <si>
-    <t>6/12/2024</t>
+    <t>5/8/2024</t>
+  </si>
+  <si>
+    <t>8/12/2024</t>
   </si>
   <si>
     <t>Ông</t>
@@ -121,6 +121,9 @@
     <t>Giảng viên</t>
   </si>
   <si>
+    <t>988710727</t>
+  </si>
+  <si>
     <t>22010000163 915</t>
   </si>
   <si>
@@ -136,13 +139,70 @@
     <t>chín triệu chín trăm nghìn đồng</t>
   </si>
   <si>
-    <t>Dương Văn Mạnh</t>
-  </si>
-  <si>
-    <t>11/2/1978</t>
-  </si>
-  <si>
-    <t>035078000000</t>
+    <t>Nguyễn Hoàng Minh An</t>
+  </si>
+  <si>
+    <t>7/2/1978</t>
+  </si>
+  <si>
+    <t>035078000253</t>
+  </si>
+  <si>
+    <t>bốn triệu ba trăm nghìn đồng</t>
+  </si>
+  <si>
+    <t>bốn trăm ba mươi nghìn đồng</t>
+  </si>
+  <si>
+    <t>ba triệu tám trăm bảy mươi nghìn đồng</t>
+  </si>
+  <si>
+    <t>Đặng Thị Kim Anh</t>
+  </si>
+  <si>
+    <t>12/2/1978</t>
+  </si>
+  <si>
+    <t>00207800098003</t>
+  </si>
+  <si>
+    <t>mười triệu đồng</t>
+  </si>
+  <si>
+    <t>một triệu đồng</t>
+  </si>
+  <si>
+    <t>chín triệu đồng</t>
+  </si>
+  <si>
+    <t>Đỗ Thái Dương</t>
+  </si>
+  <si>
+    <t>30/10/2024</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Hà Nội</t>
+  </si>
+  <si>
+    <t>huedm.c3chuyen@thainguyen.edu.vn</t>
+  </si>
+  <si>
+    <t>Thạc sĩ</t>
+  </si>
+  <si>
+    <t>giảng viên</t>
+  </si>
+  <si>
+    <t>334553232</t>
+  </si>
+  <si>
+    <t>0325266412</t>
+  </si>
+  <si>
+    <t>mb bank</t>
   </si>
   <si>
     <t>sáu triệu năm trăm nghìn đồng</t>
@@ -152,60 +212,6 @@
   </si>
   <si>
     <t>năm triệu tám trăm năm mươi nghìn đồng</t>
-  </si>
-  <si>
-    <t>Đặng Thị Kim Anh</t>
-  </si>
-  <si>
-    <t>12/2/1978</t>
-  </si>
-  <si>
-    <t>00207800098003</t>
-  </si>
-  <si>
-    <t>mười triệu đồng</t>
-  </si>
-  <si>
-    <t>một triệu đồng</t>
-  </si>
-  <si>
-    <t>chín triệu đồng</t>
-  </si>
-  <si>
-    <t>Đỗ Thái Dương</t>
-  </si>
-  <si>
-    <t>31/10/2024</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>Hà Nội</t>
-  </si>
-  <si>
-    <t>huedm.c3chuyen@thainguyen.edu.vn</t>
-  </si>
-  <si>
-    <t>Thạc sĩ</t>
-  </si>
-  <si>
-    <t>giảng viên</t>
-  </si>
-  <si>
-    <t>0325266412</t>
-  </si>
-  <si>
-    <t>mb bank</t>
-  </si>
-  <si>
-    <t>bốn triệu ba trăm nghìn đồng</t>
-  </si>
-  <si>
-    <t>bốn trăm ba mươi nghìn đồng</t>
-  </si>
-  <si>
-    <t>ba triệu tám trăm bảy mươi nghìn đồng</t>
   </si>
   <si>
     <t>Đoàn Minh Phương</t>
@@ -751,14 +757,14 @@
       <c r="N2" s="2">
         <v>4</v>
       </c>
-      <c r="O2" s="2">
-        <v>988710727</v>
+      <c r="O2" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R2" s="2">
         <v>110</v>
@@ -767,19 +773,19 @@
         <v>11000000</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U2" s="2">
         <v>1100000</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="W2" s="2">
         <v>9900000</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Y2" s="2" t="s">
         <v>26</v>
@@ -799,13 +805,13 @@
         <v>27</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>31</v>
@@ -828,35 +834,35 @@
       <c r="N3" s="2">
         <v>4</v>
       </c>
-      <c r="O3" s="2">
-        <v>988710727</v>
+      <c r="O3" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R3" s="2">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="S3" s="2">
-        <v>6500000</v>
+        <v>4300000</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="U3" s="2">
-        <v>650000</v>
+        <v>430000</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="W3" s="2">
-        <v>5850000</v>
+        <v>3870000</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Y3" s="2" t="s">
         <v>26</v>
@@ -876,13 +882,13 @@
         <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>31</v>
@@ -905,14 +911,14 @@
       <c r="N4" s="2">
         <v>4</v>
       </c>
-      <c r="O4" s="2">
-        <v>988710727</v>
+      <c r="O4" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R4" s="2">
         <v>100</v>
@@ -921,19 +927,19 @@
         <v>10000000</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="U4" s="2">
         <v>1000000</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="W4" s="2">
         <v>9000000</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Y4" s="2" t="s">
         <v>26</v>
@@ -953,64 +959,64 @@
         <v>27</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K5" s="2">
         <v>0</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="N5" s="2">
         <v>4</v>
       </c>
-      <c r="O5" s="2">
-        <v>334553232</v>
+      <c r="O5" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="R5" s="2">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="S5" s="2">
-        <v>4300000</v>
+        <v>6500000</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="U5" s="2">
-        <v>430000</v>
+        <v>650000</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="W5" s="2">
-        <v>3870000</v>
+        <v>5850000</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="Y5" s="2" t="s">
         <v>26</v>
@@ -1030,13 +1036,13 @@
         <v>27</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>31</v>
@@ -1059,14 +1065,14 @@
       <c r="N6" s="2">
         <v>4</v>
       </c>
-      <c r="O6" s="2">
-        <v>988710727</v>
+      <c r="O6" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R6" s="2">
         <v>65</v>
@@ -1075,19 +1081,19 @@
         <v>6500000</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="U6" s="2">
         <v>650000</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="W6" s="2">
         <v>5850000</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="Y6" s="2" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
thêm dấu phẩy ở tiền
</commit_message>
<xml_diff>
--- a/src/public/exports/hopdonggvmList.xlsx
+++ b/src/public/exports/hopdonggvmList.xlsx
@@ -127,13 +127,13 @@
     <t>BIDV, chi nhánh Thăng Long</t>
   </si>
   <si>
-    <t>mười một triệu đồng</t>
-  </si>
-  <si>
-    <t>một triệu một trăm nghìn đồng</t>
-  </si>
-  <si>
-    <t>chín triệu chín trăm nghìn đồng</t>
+    <t>Mười một triệu đồng</t>
+  </si>
+  <si>
+    <t>Một triệu một trăm nghìn đồng</t>
+  </si>
+  <si>
+    <t>Chín triệu chín trăm nghìn đồng</t>
   </si>
   <si>
     <t>Nguyễn Hoàng Minh An</t>
@@ -145,13 +145,13 @@
     <t>035078000253</t>
   </si>
   <si>
-    <t>bốn triệu ba trăm nghìn đồng</t>
-  </si>
-  <si>
-    <t>bốn trăm ba mươi nghìn đồng</t>
-  </si>
-  <si>
-    <t>ba triệu tám trăm bảy mươi nghìn đồng</t>
+    <t>Bốn triệu ba trăm nghìn đồng</t>
+  </si>
+  <si>
+    <t>Bốn trăm ba mươi nghìn đồng</t>
+  </si>
+  <si>
+    <t>Ba triệu tám trăm bảy mươi nghìn đồng</t>
   </si>
   <si>
     <t>Đặng Thị Kim Anh</t>
@@ -163,13 +163,13 @@
     <t>00207800098003</t>
   </si>
   <si>
-    <t>mười triệu đồng</t>
-  </si>
-  <si>
-    <t>một triệu đồng</t>
-  </si>
-  <si>
-    <t>chín triệu đồng</t>
+    <t>Mười triệu đồng</t>
+  </si>
+  <si>
+    <t>Một triệu đồng</t>
+  </si>
+  <si>
+    <t>Chín triệu đồng</t>
   </si>
   <si>
     <t>Đỗ Thái Dương</t>
@@ -199,13 +199,13 @@
     <t>mb bank</t>
   </si>
   <si>
-    <t>sáu triệu năm trăm nghìn đồng</t>
-  </si>
-  <si>
-    <t>sáu trăm năm mươi nghìn đồng</t>
-  </si>
-  <si>
-    <t>năm triệu tám trăm năm mươi nghìn đồng</t>
+    <t>Sáu triệu năm trăm nghìn đồng</t>
+  </si>
+  <si>
+    <t>Sáu trăm năm mươi nghìn đồng</t>
+  </si>
+  <si>
+    <t>Năm triệu tám trăm năm mươi nghìn đồng</t>
   </si>
   <si>
     <t>Đoàn Minh Phương</t>
@@ -260,12 +260,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,474 +627,474 @@
     <col min="15" max="16" width="15" customWidth="1"/>
     <col min="17" max="17" width="20" customWidth="1"/>
     <col min="18" max="18" width="10" customWidth="1"/>
-    <col min="19" max="19" width="15" customWidth="1"/>
+    <col min="19" max="19" width="15" style="1" customWidth="1"/>
     <col min="20" max="20" width="30" customWidth="1"/>
-    <col min="21" max="21" width="15" customWidth="1"/>
+    <col min="21" max="21" width="15" style="1" customWidth="1"/>
     <col min="22" max="22" width="30" customWidth="1"/>
-    <col min="23" max="23" width="15" customWidth="1"/>
+    <col min="23" max="23" width="15" style="1" customWidth="1"/>
     <col min="24" max="24" width="30" customWidth="1"/>
     <col min="25" max="25" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="4">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="4">
         <v>2147483647</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="4">
         <v>4</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="4">
         <v>988710727</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="R2" s="2">
+      <c r="R2" s="4">
         <v>110</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="5">
         <v>11000000</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="T2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2" s="5">
         <v>1100000</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="V2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="W2" s="2">
+      <c r="W2" s="5">
         <v>9900000</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="X2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Y2" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="4">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="4">
         <v>2147483647</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="4">
         <v>4</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3" s="4">
         <v>988710727</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="P3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="Q3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="2">
+      <c r="R3" s="4">
         <v>43</v>
       </c>
-      <c r="S3" s="2">
+      <c r="S3" s="5">
         <v>4300000</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="T3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="U3" s="2">
+      <c r="U3" s="5">
         <v>430000</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="V3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="W3" s="2">
+      <c r="W3" s="5">
         <v>3870000</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="X3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="Y3" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="4">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="4">
         <v>2147483647</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="4">
         <v>4</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="4">
         <v>988710727</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="Q4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="R4" s="2">
+      <c r="R4" s="4">
         <v>100</v>
       </c>
-      <c r="S4" s="2">
+      <c r="S4" s="5">
         <v>10000000</v>
       </c>
-      <c r="T4" s="2" t="s">
+      <c r="T4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="U4" s="2">
+      <c r="U4" s="5">
         <v>1000000</v>
       </c>
-      <c r="V4" s="2" t="s">
+      <c r="V4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="W4" s="2">
+      <c r="W4" s="5">
         <v>9000000</v>
       </c>
-      <c r="X4" s="2" t="s">
+      <c r="X4" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="Y4" s="2" t="s">
+      <c r="Y4" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="4">
         <v>1</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="4">
         <v>0</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="4">
         <v>4</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="4">
         <v>334553232</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="P5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="Q5" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="R5" s="2">
+      <c r="R5" s="4">
         <v>65</v>
       </c>
-      <c r="S5" s="2">
+      <c r="S5" s="5">
         <v>6500000</v>
       </c>
-      <c r="T5" s="2" t="s">
+      <c r="T5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="U5" s="2">
+      <c r="U5" s="5">
         <v>650000</v>
       </c>
-      <c r="V5" s="2" t="s">
+      <c r="V5" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="W5" s="2">
+      <c r="W5" s="5">
         <v>5850000</v>
       </c>
-      <c r="X5" s="2" t="s">
+      <c r="X5" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="Y5" s="2" t="s">
+      <c r="Y5" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="4">
         <v>1</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="4">
         <v>2147483647</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="4">
         <v>4</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="4">
         <v>988710727</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="P6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="Q6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="R6" s="2">
+      <c r="R6" s="4">
         <v>65</v>
       </c>
-      <c r="S6" s="2">
+      <c r="S6" s="5">
         <v>6500000</v>
       </c>
-      <c r="T6" s="2" t="s">
+      <c r="T6" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="U6" s="2">
+      <c r="U6" s="5">
         <v>650000</v>
       </c>
-      <c r="V6" s="2" t="s">
+      <c r="V6" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="W6" s="2">
+      <c r="W6" s="5">
         <v>5850000</v>
       </c>
-      <c r="X6" s="2" t="s">
+      <c r="X6" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="Y6" s="2" t="s">
+      <c r="Y6" s="4" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>